<commit_message>
time is now static
for each run will only use HHMM of when run started

minor bug fix
</commit_message>
<xml_diff>
--- a/data/steel/factories/IBF_factory-LC.xlsx
+++ b/data/steel/factories/IBF_factory-LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB937B-5BE5-2A4D-9D7F-7959714B6C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89A87E5-F8D7-6F47-A3B6-9A377673C149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="21080" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16420" yWindow="820" windowWidth="21080" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chains" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="71">
   <si>
     <t>Inflow</t>
   </si>
@@ -668,7 +668,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +860,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1545,30 +1545,9 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" t="s">
-        <v>24</v>
-      </c>
+      <c r="C26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>